<commit_message>
Working on 2-handed weapons
</commit_message>
<xml_diff>
--- a/HourRegistration.xlsx
+++ b/HourRegistration.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\GitHub\Repositories\PersonalPortfolio_Q3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79551CF2-B4EE-4731-957A-952B4DFC1008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048D45AE-880A-44AE-9961-A22780C3E580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-195" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>Learning goal 1</t>
   </si>
@@ -61,6 +70,30 @@
   </si>
   <si>
     <t>Random enemy spawning, player canvas, shop canvas</t>
+  </si>
+  <si>
+    <t>Fixed controller behaviour. NPC model add, gun functionality</t>
+  </si>
+  <si>
+    <t>9.15 - 16.00</t>
+  </si>
+  <si>
+    <t>10.30 - 12.00</t>
+  </si>
+  <si>
+    <t>Fixed enemy animations</t>
+  </si>
+  <si>
+    <t>10.15 - 12.30</t>
+  </si>
+  <si>
+    <t>13.30 - 17.00</t>
+  </si>
+  <si>
+    <t>Worked on gun system</t>
+  </si>
+  <si>
+    <t>9.00 - 14.00</t>
   </si>
 </sst>
 </file>
@@ -379,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="M29" sqref="M29:N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,6 +496,167 @@
         <v>11</v>
       </c>
     </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>44649</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6">
+        <v>6.75</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>44651</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>1.5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>44655</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8">
+        <v>2.15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>44655</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9">
+        <v>3.5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>44656</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>44657</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>44658</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>44659</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>44662</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>44663</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>44664</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>44665</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>44666</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <f>SUM(D3:D29)</f>
+        <v>65.400000000000006</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Working on enemy FSM
</commit_message>
<xml_diff>
--- a/HourRegistration.xlsx
+++ b/HourRegistration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\GitHub\Repositories\PersonalPortfolio_Q3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048D45AE-880A-44AE-9961-A22780C3E580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C57EF1-B1C1-4165-B601-234B671F9F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>Learning goal 1</t>
   </si>
@@ -94,6 +94,24 @@
   </si>
   <si>
     <t>9.00 - 14.00</t>
+  </si>
+  <si>
+    <t>20.00 - 21.00</t>
+  </si>
+  <si>
+    <t>Worked on enemy FSM</t>
+  </si>
+  <si>
+    <t>10.00 - 12.00</t>
+  </si>
+  <si>
+    <t>9.00 - 11.00</t>
+  </si>
+  <si>
+    <t>9.30 - 12.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -415,7 +433,7 @@
   <dimension ref="A1:R30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29:N30"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,51 +572,57 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>44656</v>
+        <v>44659</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>44657</v>
+        <v>44660</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D11">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>44658</v>
+        <v>44661</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D12">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>44659</v>
+        <v>44662</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>44662</v>
+        <v>44663</v>
       </c>
       <c r="B14" t="s">
         <v>19</v>
@@ -609,7 +633,7 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>44663</v>
+        <v>44664</v>
       </c>
       <c r="B15" t="s">
         <v>19</v>
@@ -620,7 +644,7 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>44664</v>
+        <v>44665</v>
       </c>
       <c r="B16" t="s">
         <v>19</v>
@@ -629,9 +653,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>44665</v>
+        <v>44666</v>
       </c>
       <c r="B17" t="s">
         <v>19</v>
@@ -640,21 +664,57 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>44666</v>
+        <v>44667</v>
       </c>
       <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>44669</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>44670</v>
+      </c>
+      <c r="B20" t="s">
         <v>19</v>
       </c>
-      <c r="D18">
+      <c r="D20">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>44671</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D30">
         <f>SUM(D3:D29)</f>
-        <v>65.400000000000006</v>
+        <v>62.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enemy waypoint system. Added patrol state.
</commit_message>
<xml_diff>
--- a/HourRegistration.xlsx
+++ b/HourRegistration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\GitHub\Repositories\PersonalPortfolio_Q3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C57EF1-B1C1-4165-B601-234B671F9F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C922CEC-3E1C-43A6-8F03-D8FE6D12EFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-195" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>Learning goal 1</t>
   </si>
@@ -105,13 +105,31 @@
     <t>10.00 - 12.00</t>
   </si>
   <si>
-    <t>9.00 - 11.00</t>
-  </si>
-  <si>
-    <t>9.30 - 12.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
+    <t>9.30 - 15.00</t>
+  </si>
+  <si>
+    <t>Enemy FSM, sound</t>
+  </si>
+  <si>
+    <t>Level design</t>
+  </si>
+  <si>
+    <t>10.00  - 12.30</t>
+  </si>
+  <si>
+    <t>Level design, background music player</t>
+  </si>
+  <si>
+    <t>Continuing for redo. Refining enemy behaviour</t>
+  </si>
+  <si>
+    <t>9.00 - 12.00</t>
+  </si>
+  <si>
+    <t>14.30 - 16.30</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Working on gunplay</t>
   </si>
 </sst>
 </file>
@@ -430,15 +448,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R30"/>
+  <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -446,7 +464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -465,14 +483,14 @@
       <c r="P2" t="s">
         <v>3</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>4</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44640</v>
       </c>
@@ -485,8 +503,9 @@
       <c r="E3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44641</v>
       </c>
@@ -500,7 +519,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44642</v>
       </c>
@@ -514,7 +533,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44649</v>
       </c>
@@ -528,7 +547,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44651</v>
       </c>
@@ -542,7 +561,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44655</v>
       </c>
@@ -556,7 +575,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44655</v>
       </c>
@@ -570,7 +589,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44659</v>
       </c>
@@ -584,7 +603,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44660</v>
       </c>
@@ -598,31 +617,37 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>44661</v>
+        <v>44662</v>
       </c>
       <c r="B12" t="s">
         <v>23</v>
       </c>
       <c r="D12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+        <v>5.5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>44662</v>
+        <v>44663</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D13">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>44663</v>
+        <v>44664</v>
       </c>
       <c r="B14" t="s">
         <v>19</v>
@@ -630,91 +655,65 @@
       <c r="D14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>44664</v>
+        <v>44665</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>44665</v>
+        <v>44699</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D16">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>44666</v>
+        <v>44700</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D17">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>44667</v>
-      </c>
-      <c r="B18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18">
-        <v>2</v>
-      </c>
-      <c r="E18" t="s">
-        <v>25</v>
-      </c>
+      <c r="A18" s="1"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>44669</v>
-      </c>
-      <c r="B19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19">
-        <v>2.5</v>
-      </c>
+      <c r="A19" s="1"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>44670</v>
-      </c>
-      <c r="B20" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>44671</v>
-      </c>
-      <c r="B21" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D30">
-        <f>SUM(D3:D29)</f>
-        <v>62.4</v>
+      <c r="A20" s="1"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <f>SUM(D3:D28)</f>
+        <v>46.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bullet pooling. Shop UI. Shop item tweening
</commit_message>
<xml_diff>
--- a/HourRegistration.xlsx
+++ b/HourRegistration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\GitHub\Repositories\PersonalPortfolio_Q3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786B3D09-F2C0-436B-8699-145D732504BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C580C34C-30C9-4D3C-992F-41C1FDEB5A92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-195" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>Learning goal 1</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>Worked on level, shop UI functionality</t>
+  </si>
+  <si>
+    <t>14.00 - 15.30</t>
+  </si>
+  <si>
+    <t>Worked on bullet pooling, shop functionality</t>
   </si>
 </sst>
 </file>
@@ -469,7 +475,7 @@
   <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S25" sqref="S25"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,10 +767,24 @@
         <v>37</v>
       </c>
     </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>44706</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21">
+        <v>1.5</v>
+      </c>
+      <c r="E21" t="s">
+        <v>39</v>
+      </c>
+    </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D29">
         <f>SUM(D3:D28)</f>
-        <v>53.5</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed pistol & rifle shooting
</commit_message>
<xml_diff>
--- a/HourRegistration.xlsx
+++ b/HourRegistration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\GitHub\Repositories\PersonalPortfolio_Q3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D88FF656-D9E6-4E0C-852D-D8EBA476AEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E081B02-9300-4BA3-997C-36B5D2AFD812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-195" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-195" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
   <si>
     <t>Learning goal 1</t>
   </si>
@@ -150,13 +150,28 @@
     <t>Worked on level, shop UI functionality</t>
   </si>
   <si>
-    <t>14.00 - 15.30</t>
-  </si>
-  <si>
-    <t>Worked on bullet pooling, shop functionality</t>
-  </si>
-  <si>
     <t>9.45 - 12.00</t>
+  </si>
+  <si>
+    <t>Shop functionality</t>
+  </si>
+  <si>
+    <t>14.00 - 14.45</t>
+  </si>
+  <si>
+    <t>14.45 - 15.30</t>
+  </si>
+  <si>
+    <t>Object pooling</t>
+  </si>
+  <si>
+    <t>Finalized level design</t>
+  </si>
+  <si>
+    <t>14.00 - 17.00a</t>
+  </si>
+  <si>
+    <t>Polishing gunplay</t>
   </si>
 </sst>
 </file>
@@ -478,7 +493,7 @@
   <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,7 +545,18 @@
       <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="1"/>
+      <c r="O3" s="1">
+        <v>44706</v>
+      </c>
+      <c r="P3" t="s">
+        <v>41</v>
+      </c>
+      <c r="R3">
+        <v>0.75</v>
+      </c>
+      <c r="S3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -714,7 +740,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44700</v>
       </c>
@@ -728,7 +754,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44701</v>
       </c>
@@ -742,7 +768,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44704</v>
       </c>
@@ -756,7 +782,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44705</v>
       </c>
@@ -770,26 +796,26 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44706</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D21">
-        <v>1.5</v>
+        <v>0.75</v>
       </c>
       <c r="E21" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44708</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D22">
         <v>2.25</v>
@@ -798,10 +824,42 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>44711</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23">
+        <v>2.25</v>
+      </c>
+      <c r="E23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>44712</v>
+      </c>
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D29">
         <f>SUM(D3:D28)</f>
-        <v>57.25</v>
+        <v>61.75</v>
+      </c>
+      <c r="R29">
+        <f>SUM(R3:R28)</f>
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reverted back to SRP.
</commit_message>
<xml_diff>
--- a/HourRegistration.xlsx
+++ b/HourRegistration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\GitHub\Repositories\PersonalPortfolio_Q3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215EEA6B-6615-4EC4-B7CB-76975989FA39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1987C34B-25C9-4644-81B3-E3E614BF2403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-195" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -180,10 +180,10 @@
     <t>Fixing shop bugs</t>
   </si>
   <si>
-    <t>12.00 - 13.00</t>
-  </si>
-  <si>
-    <t>Tested object pooling, tried out occlusion culling</t>
+    <t>12.00 - 13.30</t>
+  </si>
+  <si>
+    <t>Started writing optimization research doc. Tried upgrading to HDRP (didn't work, asset pack incompatible)</t>
   </si>
 </sst>
 </file>
@@ -505,7 +505,7 @@
   <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,7 +590,7 @@
         <v>48</v>
       </c>
       <c r="R4">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="S4" t="s">
         <v>49</v>
@@ -911,7 +911,7 @@
       </c>
       <c r="R29">
         <f>SUM(R3:R28)</f>
-        <v>1.75</v>
+        <v>2.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on test research doc, lighting data
</commit_message>
<xml_diff>
--- a/HourRegistration.xlsx
+++ b/HourRegistration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\GitHub\Repositories\PersonalPortfolio_Q3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1987C34B-25C9-4644-81B3-E3E614BF2403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75CA7A1-7D93-484A-8418-DAAC83F56E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-195" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
   <si>
     <t>Learning goal 1</t>
   </si>
@@ -184,6 +184,12 @@
   </si>
   <si>
     <t>Started writing optimization research doc. Tried upgrading to HDRP (didn't work, asset pack incompatible)</t>
+  </si>
+  <si>
+    <t>12.45 - 15.00</t>
+  </si>
+  <si>
+    <t>Lighting, research doc</t>
   </si>
 </sst>
 </file>
@@ -505,7 +511,7 @@
   <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,6 +615,18 @@
       <c r="E5" t="s">
         <v>11</v>
       </c>
+      <c r="O5" s="1">
+        <v>44725</v>
+      </c>
+      <c r="P5" t="s">
+        <v>50</v>
+      </c>
+      <c r="R5">
+        <v>2.25</v>
+      </c>
+      <c r="S5" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -903,6 +921,9 @@
       <c r="E26" t="s">
         <v>45</v>
       </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D29">
@@ -911,7 +932,7 @@
       </c>
       <c r="R29">
         <f>SUM(R3:R28)</f>
-        <v>2.25</v>
+        <v>4.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testing Github PDF displaying
</commit_message>
<xml_diff>
--- a/HourRegistration.xlsx
+++ b/HourRegistration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\GitHub\Repositories\PersonalPortfolio_Q3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75CA7A1-7D93-484A-8418-DAAC83F56E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1DAC56-5E63-4F5C-B745-0D5324E70FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-195" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
   <si>
     <t>Learning goal 1</t>
   </si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t>Lighting, research doc</t>
+  </si>
+  <si>
+    <t>Writing out tests in research doc.</t>
   </si>
 </sst>
 </file>
@@ -511,7 +514,7 @@
   <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,6 +644,18 @@
       <c r="E6" t="s">
         <v>12</v>
       </c>
+      <c r="O6" s="1">
+        <v>44726</v>
+      </c>
+      <c r="P6" t="s">
+        <v>29</v>
+      </c>
+      <c r="R6">
+        <v>3</v>
+      </c>
+      <c r="S6" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -932,7 +947,7 @@
       </c>
       <c r="R29">
         <f>SUM(R3:R28)</f>
-        <v>4.5</v>
+        <v>7.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalized Occlusion Culling test. Prepared Object Pooling test.
</commit_message>
<xml_diff>
--- a/HourRegistration.xlsx
+++ b/HourRegistration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\GitHub\Repositories\PersonalPortfolio_Q3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1DAC56-5E63-4F5C-B745-0D5324E70FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22DF0A00-E69B-40E2-BA42-7ABA135ADD59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-195" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="57">
   <si>
     <t>Learning goal 1</t>
   </si>
@@ -193,6 +193,18 @@
   </si>
   <si>
     <t>Writing out tests in research doc.</t>
+  </si>
+  <si>
+    <t>13.30 - 15.00</t>
+  </si>
+  <si>
+    <t>Working on occlusion culling test.</t>
+  </si>
+  <si>
+    <t>8.30 - 11.30</t>
+  </si>
+  <si>
+    <t>Occlusion culling test. Processing data. Prepare object pooling test.</t>
   </si>
 </sst>
 </file>
@@ -514,7 +526,7 @@
   <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,6 +682,18 @@
       <c r="E7" t="s">
         <v>15</v>
       </c>
+      <c r="O7" s="1">
+        <v>44727</v>
+      </c>
+      <c r="P7" t="s">
+        <v>53</v>
+      </c>
+      <c r="R7">
+        <v>1.5</v>
+      </c>
+      <c r="S7" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -683,6 +707,18 @@
       </c>
       <c r="E8" t="s">
         <v>18</v>
+      </c>
+      <c r="O8" s="1">
+        <v>44728</v>
+      </c>
+      <c r="P8" t="s">
+        <v>55</v>
+      </c>
+      <c r="R8">
+        <v>2.5</v>
+      </c>
+      <c r="S8" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -947,7 +983,7 @@
       </c>
       <c r="R29">
         <f>SUM(R3:R28)</f>
-        <v>7.5</v>
+        <v>11.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Performed object pooling test. Working on sync vs async loading test
</commit_message>
<xml_diff>
--- a/HourRegistration.xlsx
+++ b/HourRegistration.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\GitHub\Repositories\PersonalPortfolio_Q3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22DF0A00-E69B-40E2-BA42-7ABA135ADD59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F076F0D6-D435-49CA-B2EA-B514A933E01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="60">
   <si>
     <t>Learning goal 1</t>
   </si>
@@ -205,6 +205,15 @@
   </si>
   <si>
     <t>Occlusion culling test. Processing data. Prepare object pooling test.</t>
+  </si>
+  <si>
+    <t>10.15 - 12.15</t>
+  </si>
+  <si>
+    <t>Object pooling test.</t>
+  </si>
+  <si>
+    <t>8.00 - 12.00</t>
   </si>
 </sst>
 </file>
@@ -526,7 +535,7 @@
   <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+      <selection activeCell="Y27" sqref="Y27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,6 +743,18 @@
       <c r="E9" t="s">
         <v>18</v>
       </c>
+      <c r="O9" s="1">
+        <v>44746</v>
+      </c>
+      <c r="P9" t="s">
+        <v>57</v>
+      </c>
+      <c r="R9">
+        <v>2</v>
+      </c>
+      <c r="S9" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -748,6 +769,15 @@
       <c r="E10" t="s">
         <v>21</v>
       </c>
+      <c r="O10" s="1">
+        <v>44746</v>
+      </c>
+      <c r="P10" t="s">
+        <v>8</v>
+      </c>
+      <c r="R10">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -761,6 +791,15 @@
       </c>
       <c r="E11" t="s">
         <v>21</v>
+      </c>
+      <c r="O11" s="1">
+        <v>44747</v>
+      </c>
+      <c r="P11" t="s">
+        <v>59</v>
+      </c>
+      <c r="R11">
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -983,7 +1022,7 @@
       </c>
       <c r="R29">
         <f>SUM(R3:R28)</f>
-        <v>11.5</v>
+        <v>20.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Object pooling, async scene loading tests. Prepared batching tests.
</commit_message>
<xml_diff>
--- a/HourRegistration.xlsx
+++ b/HourRegistration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\GitHub\Repositories\PersonalPortfolio_Q3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F076F0D6-D435-49CA-B2EA-B514A933E01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D06125-E528-4DA9-9EE6-6300FA38BF07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
   <si>
     <t>Learning goal 1</t>
   </si>
@@ -214,6 +214,12 @@
   </si>
   <si>
     <t>8.00 - 12.00</t>
+  </si>
+  <si>
+    <t>16.00 - 18.00</t>
+  </si>
+  <si>
+    <t>Performed scene loading test. Performed batching test.</t>
   </si>
 </sst>
 </file>
@@ -535,7 +541,7 @@
   <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y27" sqref="Y27"/>
+      <selection activeCell="T33" sqref="T33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,10 +779,13 @@
         <v>44746</v>
       </c>
       <c r="P10" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="R10">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="S10" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -1022,7 +1031,7 @@
       </c>
       <c r="R29">
         <f>SUM(R3:R28)</f>
-        <v>20.5</v>
+        <v>19.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ran and processed all tests.
</commit_message>
<xml_diff>
--- a/HourRegistration.xlsx
+++ b/HourRegistration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\GitHub\Repositories\PersonalPortfolio_Q3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D06125-E528-4DA9-9EE6-6300FA38BF07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4862F17-C003-4932-BFAC-7986B7641350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-195" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="65">
   <si>
     <t>Learning goal 1</t>
   </si>
@@ -213,13 +213,22 @@
     <t>Object pooling test.</t>
   </si>
   <si>
-    <t>8.00 - 12.00</t>
-  </si>
-  <si>
     <t>16.00 - 18.00</t>
   </si>
   <si>
     <t>Performed scene loading test. Performed batching test.</t>
+  </si>
+  <si>
+    <t>Redoing all previous tests. Didn’t realize vsync was on... Performed graphics quality test. Performed lighting test.</t>
+  </si>
+  <si>
+    <t>8.15 - 15.15</t>
+  </si>
+  <si>
+    <t>17.00 - 20.30</t>
+  </si>
+  <si>
+    <t>Finalized game. Preparing handin.</t>
   </si>
 </sst>
 </file>
@@ -541,7 +550,7 @@
   <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T33" sqref="T33"/>
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,13 +788,13 @@
         <v>44746</v>
       </c>
       <c r="P10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R10">
         <v>2</v>
       </c>
       <c r="S10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -805,10 +814,13 @@
         <v>44747</v>
       </c>
       <c r="P11" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="R11">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="S11" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -1022,16 +1034,27 @@
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
+      <c r="A27" s="1">
+        <v>44747</v>
+      </c>
+      <c r="B27" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27">
+        <v>3.5</v>
+      </c>
+      <c r="E27" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D29">
         <f>SUM(D3:D28)</f>
-        <v>65.75</v>
+        <v>69.25</v>
       </c>
       <c r="R29">
         <f>SUM(R3:R28)</f>
-        <v>19.5</v>
+        <v>22.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>